<commit_message>
Font Icons Mapping Obj
</commit_message>
<xml_diff>
--- a/src/assets/MyHealthRecords_App.xlsx
+++ b/src/assets/MyHealthRecords_App.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GK-96\Desktop\MyHealthRecords.gr_App\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A4D795-DD37-4661-B0FB-837F72F7D939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B934E339-FC9D-443D-89DD-A9E6A98D1211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33017" yWindow="-4277" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{CCBED421-2667-4BAF-8A4C-3918BA6E9EF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CCBED421-2667-4BAF-8A4C-3918BA6E9EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Σε επόμενο στάδιο της εφαρμογής θα χρειάζεται επιβεβαίωση του λογαριασμού μέσα σε 15 μέρες. Υπό διαφορετικές συνθήκες η πρόσβαση στο λογαριασμό δε θα είναι δυνατή</t>
   </si>
   <si>
-    <t>Στην εφαρμογή θα γίνει χρήση σχεσιακής βάσης δεδομένων</t>
-  </si>
-  <si>
     <t>α/α</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t xml:space="preserve">float </t>
+  </si>
+  <si>
+    <t>Στην εφαρμογή θα γίνει χρήση μη σχεσιακής βάσης δεδομένων</t>
   </si>
 </sst>
 </file>
@@ -787,6 +787,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -805,29 +823,11 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J8" s="39" t="s">
         <v>1</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="17" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J17" s="39" t="s">
         <v>2</v>
@@ -1929,7 +1929,7 @@
   <dimension ref="G2:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,7 +1939,7 @@
   <sheetData>
     <row r="2" spans="7:22" x14ac:dyDescent="0.25">
       <c r="I2" s="39" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
@@ -1949,13 +1949,13 @@
     </row>
     <row r="5" spans="7:22" x14ac:dyDescent="0.25">
       <c r="I5" s="42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="42"/>
       <c r="K5" s="42"/>
       <c r="L5" s="42"/>
       <c r="O5" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P5" s="39"/>
       <c r="Q5" s="39"/>
@@ -1967,16 +1967,16 @@
     </row>
     <row r="6" spans="7:22" x14ac:dyDescent="0.25">
       <c r="I6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1989,25 +1989,25 @@
     </row>
     <row r="7" spans="7:22" x14ac:dyDescent="0.25">
       <c r="H7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="5">
         <v>1</v>
       </c>
       <c r="J7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="O7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P7" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q7" s="43"/>
       <c r="R7" s="43"/>
@@ -2021,13 +2021,13 @@
         <v>2</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="43"/>
@@ -2043,13 +2043,13 @@
         <v>3</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="43"/>
@@ -2065,13 +2065,13 @@
         <v>4</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="43"/>
@@ -2087,13 +2087,13 @@
         <v>5</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="43"/>
@@ -2109,13 +2109,13 @@
         <v>6</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -2131,13 +2131,13 @@
         <v>7</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -2153,19 +2153,19 @@
         <v>8</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P14" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q14" s="45"/>
       <c r="R14" s="45"/>
@@ -2179,13 +2179,13 @@
         <v>9</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="45"/>
@@ -2198,19 +2198,19 @@
     </row>
     <row r="16" spans="7:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I16" s="4">
         <v>10</v>
       </c>
       <c r="J16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="K16" s="32" t="s">
-        <v>113</v>
-      </c>
       <c r="L16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="45"/>
@@ -2223,19 +2223,19 @@
     </row>
     <row r="17" spans="8:22" x14ac:dyDescent="0.25">
       <c r="H17" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="10">
         <v>11</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="45"/>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="20" spans="8:22" x14ac:dyDescent="0.25">
       <c r="I20" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J20" s="42"/>
       <c r="K20" s="42"/>
@@ -2284,22 +2284,22 @@
     </row>
     <row r="21" spans="8:22" x14ac:dyDescent="0.25">
       <c r="I21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="O21" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P21" s="46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q21" s="46"/>
       <c r="R21" s="46"/>
@@ -2313,13 +2313,13 @@
         <v>1</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="L22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="46"/>
@@ -2335,13 +2335,13 @@
         <v>2</v>
       </c>
       <c r="J23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="L23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="46"/>
@@ -2354,19 +2354,19 @@
     </row>
     <row r="24" spans="8:22" x14ac:dyDescent="0.25">
       <c r="H24" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I24" s="12">
         <v>3</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="46"/>
@@ -2382,13 +2382,13 @@
         <v>4</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="46"/>
@@ -2404,13 +2404,13 @@
         <v>5</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -2426,13 +2426,13 @@
         <v>6</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -2445,10 +2445,10 @@
     </row>
     <row r="28" spans="8:22" x14ac:dyDescent="0.25">
       <c r="O28" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P28" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q28" s="44"/>
       <c r="R28" s="44"/>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="30" spans="8:22" x14ac:dyDescent="0.25">
       <c r="I30" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
@@ -2485,16 +2485,16 @@
     </row>
     <row r="31" spans="8:22" x14ac:dyDescent="0.25">
       <c r="I31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="L31" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="44"/>
@@ -2510,13 +2510,13 @@
         <v>1</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="44"/>
@@ -2532,13 +2532,13 @@
         <v>2</v>
       </c>
       <c r="J33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="L33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
@@ -2554,13 +2554,13 @@
         <v>3</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -2576,19 +2576,19 @@
         <v>4</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O35" s="14">
         <v>1</v>
       </c>
       <c r="P35" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q35" s="41"/>
       <c r="R35" s="41"/>
@@ -2602,13 +2602,13 @@
         <v>5</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="41"/>
@@ -2624,13 +2624,13 @@
         <v>6</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="41"/>
@@ -2646,13 +2646,13 @@
         <v>7</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="41"/>
@@ -2668,13 +2668,13 @@
         <v>8</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="41"/>
@@ -2690,13 +2690,13 @@
         <v>9</v>
       </c>
       <c r="J40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K40" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="L40" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -2712,13 +2712,13 @@
         <v>10</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -2735,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="P42" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q42" s="41"/>
       <c r="R42" s="41"/>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="44" spans="8:22" x14ac:dyDescent="0.25">
       <c r="I44" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J44" s="29"/>
       <c r="K44" s="29"/>
@@ -2772,16 +2772,16 @@
     </row>
     <row r="45" spans="8:22" x14ac:dyDescent="0.25">
       <c r="I45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="L45" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="O45" s="1"/>
       <c r="P45" s="41"/>
@@ -2797,13 +2797,13 @@
         <v>1</v>
       </c>
       <c r="J46" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K46" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K46" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="L46" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="41"/>
@@ -2819,30 +2819,30 @@
         <v>2</v>
       </c>
       <c r="J47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K47" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="L47" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="8:22" x14ac:dyDescent="0.25">
       <c r="H48" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I48" s="7">
         <v>3</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="9:12" x14ac:dyDescent="0.25">
@@ -2850,13 +2850,13 @@
         <v>4</v>
       </c>
       <c r="J49" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K49" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="K49" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="L49" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="9:12" ht="30" x14ac:dyDescent="0.25">
@@ -2864,13 +2864,13 @@
         <v>5</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K50" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="9:12" x14ac:dyDescent="0.25">
@@ -2878,13 +2878,13 @@
         <v>6</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2911,8 +2911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288CFF48-E086-40CD-9240-0256C1A06465}">
   <dimension ref="D3:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="X31" sqref="X31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,10 +2921,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D3" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="54"/>
+      <c r="D3" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="48"/>
       <c r="F3" s="19"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -2943,8 +2943,8 @@
       <c r="U3" s="17"/>
     </row>
     <row r="4" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D4" s="55"/>
-      <c r="E4" s="56"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50"/>
       <c r="F4" s="21"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -2963,8 +2963,8 @@
       <c r="U4" s="18"/>
     </row>
     <row r="5" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D5" s="55"/>
-      <c r="E5" s="56"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="50"/>
       <c r="F5" s="21"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -2983,8 +2983,8 @@
       <c r="U5" s="18"/>
     </row>
     <row r="6" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D6" s="55"/>
-      <c r="E6" s="56"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="50"/>
       <c r="F6" s="21"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -3003,8 +3003,8 @@
       <c r="U6" s="18"/>
     </row>
     <row r="7" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D7" s="55"/>
-      <c r="E7" s="56"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
       <c r="F7" s="21"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -3063,68 +3063,68 @@
       <c r="U9" s="18"/>
     </row>
     <row r="10" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="59" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="60"/>
-      <c r="F10" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="49"/>
+      <c r="D10" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="55"/>
     </row>
     <row r="11" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D11" s="59"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="49"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="55"/>
     </row>
     <row r="12" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D12" s="59"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="49"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="54"/>
+      <c r="T12" s="54"/>
+      <c r="U12" s="55"/>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" s="20"/>
@@ -3147,68 +3147,68 @@
       <c r="U13" s="18"/>
     </row>
     <row r="14" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="51"/>
+      <c r="D14" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="57"/>
     </row>
     <row r="15" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D15" s="59"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="57"/>
     </row>
     <row r="16" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="57"/>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="20"/>
@@ -3231,68 +3231,68 @@
       <c r="U17" s="18"/>
     </row>
     <row r="18" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="49"/>
+      <c r="D18" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="52"/>
+      <c r="F18" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="55"/>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="48"/>
-      <c r="S19" s="48"/>
-      <c r="T19" s="48"/>
-      <c r="U19" s="49"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="54"/>
+      <c r="U19" s="55"/>
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D20" s="59"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="48"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="49"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
+      <c r="T20" s="54"/>
+      <c r="U20" s="55"/>
     </row>
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="20"/>
@@ -3315,68 +3315,68 @@
       <c r="U21" s="18"/>
     </row>
     <row r="22" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="60"/>
-      <c r="F22" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="48"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="48"/>
-      <c r="S22" s="48"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="49"/>
+      <c r="D22" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="52"/>
+      <c r="F22" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
+      <c r="T22" s="54"/>
+      <c r="U22" s="55"/>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D23" s="59"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="49"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
+      <c r="T23" s="54"/>
+      <c r="U23" s="55"/>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D24" s="59"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="48"/>
-      <c r="R24" s="48"/>
-      <c r="S24" s="48"/>
-      <c r="T24" s="48"/>
-      <c r="U24" s="49"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
+      <c r="T24" s="54"/>
+      <c r="U24" s="55"/>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="20"/>
@@ -3399,68 +3399,68 @@
       <c r="U25" s="18"/>
     </row>
     <row r="26" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="60"/>
-      <c r="F26" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="50"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="50"/>
-      <c r="R26" s="50"/>
-      <c r="S26" s="50"/>
-      <c r="T26" s="50"/>
-      <c r="U26" s="51"/>
+      <c r="D26" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="52"/>
+      <c r="F26" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="56"/>
+      <c r="S26" s="56"/>
+      <c r="T26" s="56"/>
+      <c r="U26" s="57"/>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="56"/>
+      <c r="S27" s="56"/>
+      <c r="T27" s="56"/>
+      <c r="U27" s="57"/>
     </row>
     <row r="28" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D28" s="59"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
-      <c r="T28" s="50"/>
-      <c r="U28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="57"/>
     </row>
     <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" s="20"/>
@@ -3483,68 +3483,68 @@
       <c r="U29" s="18"/>
     </row>
     <row r="30" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="50"/>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="50"/>
-      <c r="T30" s="50"/>
-      <c r="U30" s="51"/>
+      <c r="D30" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="52"/>
+      <c r="F30" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
+      <c r="S30" s="56"/>
+      <c r="T30" s="56"/>
+      <c r="U30" s="57"/>
     </row>
     <row r="31" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D31" s="59"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="50"/>
-      <c r="U31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
+      <c r="T31" s="56"/>
+      <c r="U31" s="57"/>
     </row>
     <row r="32" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D32" s="59"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="50"/>
-      <c r="U32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="56"/>
+      <c r="U32" s="57"/>
     </row>
     <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D33" s="20"/>
@@ -3567,68 +3567,68 @@
       <c r="U33" s="18"/>
     </row>
     <row r="34" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D34" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="60"/>
-      <c r="F34" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50"/>
-      <c r="T34" s="50"/>
-      <c r="U34" s="51"/>
+      <c r="D34" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="52"/>
+      <c r="F34" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="56"/>
+      <c r="R34" s="56"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="56"/>
+      <c r="U34" s="57"/>
     </row>
     <row r="35" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D35" s="59"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="50"/>
-      <c r="T35" s="50"/>
-      <c r="U35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
+      <c r="S35" s="56"/>
+      <c r="T35" s="56"/>
+      <c r="U35" s="57"/>
     </row>
     <row r="36" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D36" s="59"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="50"/>
-      <c r="L36" s="50"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="50"/>
-      <c r="O36" s="50"/>
-      <c r="P36" s="50"/>
-      <c r="Q36" s="50"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="50"/>
-      <c r="T36" s="50"/>
-      <c r="U36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
+      <c r="R36" s="56"/>
+      <c r="S36" s="56"/>
+      <c r="T36" s="56"/>
+      <c r="U36" s="57"/>
     </row>
     <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37" s="23"/>
@@ -3651,12 +3651,12 @@
       <c r="U37" s="18"/>
     </row>
     <row r="38" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="52"/>
+      <c r="F38" s="61" t="s">
         <v>110</v>
-      </c>
-      <c r="E38" s="60"/>
-      <c r="F38" s="61" t="s">
-        <v>111</v>
       </c>
       <c r="G38" s="62"/>
       <c r="H38" s="62"/>
@@ -3675,8 +3675,8 @@
       <c r="U38" s="63"/>
     </row>
     <row r="39" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D39" s="59"/>
-      <c r="E39" s="60"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="52"/>
       <c r="F39" s="64"/>
       <c r="G39" s="62"/>
       <c r="H39" s="62"/>
@@ -3695,8 +3695,8 @@
       <c r="U39" s="63"/>
     </row>
     <row r="40" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D40" s="59"/>
-      <c r="E40" s="60"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="52"/>
       <c r="F40" s="64"/>
       <c r="G40" s="62"/>
       <c r="H40" s="62"/>
@@ -3735,68 +3735,68 @@
       <c r="U41" s="26"/>
     </row>
     <row r="42" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D42" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="E42" s="60"/>
-      <c r="F42" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="G42" s="50"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
-      <c r="K42" s="50"/>
-      <c r="L42" s="50"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="50"/>
-      <c r="S42" s="50"/>
-      <c r="T42" s="50"/>
-      <c r="U42" s="51"/>
+      <c r="D42" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" s="52"/>
+      <c r="F42" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="56"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="56"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="56"/>
+      <c r="R42" s="56"/>
+      <c r="S42" s="56"/>
+      <c r="T42" s="56"/>
+      <c r="U42" s="57"/>
     </row>
     <row r="43" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D43" s="59"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="50"/>
-      <c r="L43" s="50"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="50"/>
-      <c r="R43" s="50"/>
-      <c r="S43" s="50"/>
-      <c r="T43" s="50"/>
-      <c r="U43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="56"/>
+      <c r="K43" s="56"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="56"/>
+      <c r="O43" s="56"/>
+      <c r="P43" s="56"/>
+      <c r="Q43" s="56"/>
+      <c r="R43" s="56"/>
+      <c r="S43" s="56"/>
+      <c r="T43" s="56"/>
+      <c r="U43" s="57"/>
     </row>
     <row r="44" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D44" s="59"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="50"/>
-      <c r="L44" s="50"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50"/>
-      <c r="R44" s="50"/>
-      <c r="S44" s="50"/>
-      <c r="T44" s="50"/>
-      <c r="U44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
+      <c r="O44" s="56"/>
+      <c r="P44" s="56"/>
+      <c r="Q44" s="56"/>
+      <c r="R44" s="56"/>
+      <c r="S44" s="56"/>
+      <c r="T44" s="56"/>
+      <c r="U44" s="57"/>
     </row>
     <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" s="23"/>
@@ -3851,12 +3851,12 @@
       <c r="U47" s="18"/>
     </row>
     <row r="48" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D48" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="54"/>
+      <c r="D48" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="48"/>
       <c r="F48" s="61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G48" s="62"/>
       <c r="H48" s="62"/>
@@ -3875,8 +3875,8 @@
       <c r="U48" s="63"/>
     </row>
     <row r="49" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D49" s="55"/>
-      <c r="E49" s="56"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="50"/>
       <c r="F49" s="64"/>
       <c r="G49" s="62"/>
       <c r="H49" s="62"/>
@@ -3895,8 +3895,8 @@
       <c r="U49" s="63"/>
     </row>
     <row r="50" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D50" s="55"/>
-      <c r="E50" s="56"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="50"/>
       <c r="F50" s="64"/>
       <c r="G50" s="62"/>
       <c r="H50" s="62"/>
@@ -3915,8 +3915,8 @@
       <c r="U50" s="63"/>
     </row>
     <row r="51" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D51" s="57"/>
-      <c r="E51" s="58"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="60"/>
       <c r="F51" s="65"/>
       <c r="G51" s="66"/>
       <c r="H51" s="66"/>
@@ -3936,11 +3936,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D3:E7"/>
-    <mergeCell ref="D10:E12"/>
-    <mergeCell ref="D18:E20"/>
-    <mergeCell ref="D22:E24"/>
-    <mergeCell ref="D26:E28"/>
     <mergeCell ref="F10:U12"/>
     <mergeCell ref="F26:U28"/>
     <mergeCell ref="F30:U32"/>
@@ -3957,6 +3952,11 @@
     <mergeCell ref="F48:U51"/>
     <mergeCell ref="F22:U24"/>
     <mergeCell ref="F18:U20"/>
+    <mergeCell ref="D3:E7"/>
+    <mergeCell ref="D10:E12"/>
+    <mergeCell ref="D18:E20"/>
+    <mergeCell ref="D22:E24"/>
+    <mergeCell ref="D26:E28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F18" r:id="rId1" xr:uid="{36619635-C56A-4186-9BF4-E751CB45AE65}"/>

</xml_diff>

<commit_message>
preparation of button functionality on Forms,Tabs
</commit_message>
<xml_diff>
--- a/src/assets/MyHealthRecords_App.xlsx
+++ b/src/assets/MyHealthRecords_App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GK-96\Desktop\MyHealthRecords.gr_App\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B934E339-FC9D-443D-89DD-A9E6A98D1211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AF972C-32C7-4064-AB0A-0F5B84C253E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CCBED421-2667-4BAF-8A4C-3918BA6E9EF5}"/>
+    <workbookView xWindow="-30686" yWindow="-3214" windowWidth="24695" windowHeight="13260" activeTab="2" xr2:uid="{CCBED421-2667-4BAF-8A4C-3918BA6E9EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -787,6 +787,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,35 +817,17 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1711,7 +1711,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493A4E62-736F-444D-A608-D31FD3AB804F}">
   <dimension ref="G2:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,10 +2921,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="48"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="19"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -2943,8 +2943,8 @@
       <c r="U3" s="17"/>
     </row>
     <row r="4" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="21"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -2963,8 +2963,8 @@
       <c r="U4" s="18"/>
     </row>
     <row r="5" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="21"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -2983,8 +2983,8 @@
       <c r="U5" s="18"/>
     </row>
     <row r="6" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="21"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -3003,8 +3003,8 @@
       <c r="U6" s="18"/>
     </row>
     <row r="7" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D7" s="49"/>
-      <c r="E7" s="50"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="21"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -3063,68 +3063,68 @@
       <c r="U9" s="18"/>
     </row>
     <row r="10" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53" t="s">
+      <c r="E10" s="60"/>
+      <c r="F10" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="54"/>
-      <c r="T10" s="54"/>
-      <c r="U10" s="55"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="49"/>
     </row>
     <row r="11" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
-      <c r="U11" s="55"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="49"/>
     </row>
     <row r="12" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D12" s="51"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="54"/>
-      <c r="T12" s="54"/>
-      <c r="U12" s="55"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="49"/>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" s="20"/>
@@ -3147,68 +3147,68 @@
       <c r="U13" s="18"/>
     </row>
     <row r="14" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53" t="s">
+      <c r="E14" s="60"/>
+      <c r="F14" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="56"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="57"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="51"/>
     </row>
     <row r="15" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="57"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="51"/>
     </row>
     <row r="16" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="57"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="50"/>
+      <c r="T16" s="50"/>
+      <c r="U16" s="51"/>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="20"/>
@@ -3231,68 +3231,68 @@
       <c r="U17" s="18"/>
     </row>
     <row r="18" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53" t="s">
+      <c r="E18" s="60"/>
+      <c r="F18" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="55"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="49"/>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="54"/>
-      <c r="S19" s="54"/>
-      <c r="T19" s="54"/>
-      <c r="U19" s="55"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="49"/>
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="54"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="54"/>
-      <c r="T20" s="54"/>
-      <c r="U20" s="55"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="49"/>
     </row>
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="20"/>
@@ -3315,68 +3315,68 @@
       <c r="U21" s="18"/>
     </row>
     <row r="22" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="51" t="s">
+      <c r="D22" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="53" t="s">
+      <c r="E22" s="60"/>
+      <c r="F22" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="54"/>
-      <c r="Q22" s="54"/>
-      <c r="R22" s="54"/>
-      <c r="S22" s="54"/>
-      <c r="T22" s="54"/>
-      <c r="U22" s="55"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="49"/>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="55"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="49"/>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="54"/>
-      <c r="T24" s="54"/>
-      <c r="U24" s="55"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="49"/>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="20"/>
@@ -3399,68 +3399,68 @@
       <c r="U25" s="18"/>
     </row>
     <row r="26" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="51" t="s">
+      <c r="D26" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="53" t="s">
+      <c r="E26" s="60"/>
+      <c r="F26" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="56"/>
-      <c r="Q26" s="56"/>
-      <c r="R26" s="56"/>
-      <c r="S26" s="56"/>
-      <c r="T26" s="56"/>
-      <c r="U26" s="57"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="51"/>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56"/>
-      <c r="S27" s="56"/>
-      <c r="T27" s="56"/>
-      <c r="U27" s="57"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="51"/>
     </row>
     <row r="28" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D28" s="51"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="56"/>
-      <c r="U28" s="57"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="51"/>
     </row>
     <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" s="20"/>
@@ -3483,68 +3483,68 @@
       <c r="U29" s="18"/>
     </row>
     <row r="30" spans="4:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="51" t="s">
+      <c r="D30" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53" t="s">
+      <c r="E30" s="60"/>
+      <c r="F30" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
-      <c r="T30" s="56"/>
-      <c r="U30" s="57"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="51"/>
     </row>
     <row r="31" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D31" s="51"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="57"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="51"/>
     </row>
     <row r="32" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D32" s="51"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="56"/>
-      <c r="S32" s="56"/>
-      <c r="T32" s="56"/>
-      <c r="U32" s="57"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="50"/>
+      <c r="S32" s="50"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="51"/>
     </row>
     <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D33" s="20"/>
@@ -3567,68 +3567,68 @@
       <c r="U33" s="18"/>
     </row>
     <row r="34" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D34" s="51" t="s">
+      <c r="D34" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="53" t="s">
+      <c r="E34" s="60"/>
+      <c r="F34" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="56"/>
-      <c r="R34" s="56"/>
-      <c r="S34" s="56"/>
-      <c r="T34" s="56"/>
-      <c r="U34" s="57"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="50"/>
+      <c r="P34" s="50"/>
+      <c r="Q34" s="50"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="50"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="51"/>
     </row>
     <row r="35" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D35" s="51"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="56"/>
-      <c r="S35" s="56"/>
-      <c r="T35" s="56"/>
-      <c r="U35" s="57"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="50"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="50"/>
+      <c r="R35" s="50"/>
+      <c r="S35" s="50"/>
+      <c r="T35" s="50"/>
+      <c r="U35" s="51"/>
     </row>
     <row r="36" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D36" s="51"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="57"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="51"/>
     </row>
     <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37" s="23"/>
@@ -3651,10 +3651,10 @@
       <c r="U37" s="18"/>
     </row>
     <row r="38" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D38" s="51" t="s">
+      <c r="D38" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="52"/>
+      <c r="E38" s="60"/>
       <c r="F38" s="61" t="s">
         <v>110</v>
       </c>
@@ -3675,8 +3675,8 @@
       <c r="U38" s="63"/>
     </row>
     <row r="39" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D39" s="51"/>
-      <c r="E39" s="52"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="64"/>
       <c r="G39" s="62"/>
       <c r="H39" s="62"/>
@@ -3695,8 +3695,8 @@
       <c r="U39" s="63"/>
     </row>
     <row r="40" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D40" s="51"/>
-      <c r="E40" s="52"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="64"/>
       <c r="G40" s="62"/>
       <c r="H40" s="62"/>
@@ -3735,68 +3735,68 @@
       <c r="U41" s="26"/>
     </row>
     <row r="42" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D42" s="51" t="s">
+      <c r="D42" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="52"/>
-      <c r="F42" s="53" t="s">
+      <c r="E42" s="60"/>
+      <c r="F42" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="56"/>
-      <c r="L42" s="56"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
-      <c r="O42" s="56"/>
-      <c r="P42" s="56"/>
-      <c r="Q42" s="56"/>
-      <c r="R42" s="56"/>
-      <c r="S42" s="56"/>
-      <c r="T42" s="56"/>
-      <c r="U42" s="57"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="50"/>
+      <c r="P42" s="50"/>
+      <c r="Q42" s="50"/>
+      <c r="R42" s="50"/>
+      <c r="S42" s="50"/>
+      <c r="T42" s="50"/>
+      <c r="U42" s="51"/>
     </row>
     <row r="43" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D43" s="51"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56"/>
-      <c r="K43" s="56"/>
-      <c r="L43" s="56"/>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
-      <c r="O43" s="56"/>
-      <c r="P43" s="56"/>
-      <c r="Q43" s="56"/>
-      <c r="R43" s="56"/>
-      <c r="S43" s="56"/>
-      <c r="T43" s="56"/>
-      <c r="U43" s="57"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="50"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="50"/>
+      <c r="P43" s="50"/>
+      <c r="Q43" s="50"/>
+      <c r="R43" s="50"/>
+      <c r="S43" s="50"/>
+      <c r="T43" s="50"/>
+      <c r="U43" s="51"/>
     </row>
     <row r="44" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D44" s="51"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
-      <c r="O44" s="56"/>
-      <c r="P44" s="56"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="56"/>
-      <c r="S44" s="56"/>
-      <c r="T44" s="56"/>
-      <c r="U44" s="57"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
+      <c r="S44" s="50"/>
+      <c r="T44" s="50"/>
+      <c r="U44" s="51"/>
     </row>
     <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" s="23"/>
@@ -3851,10 +3851,10 @@
       <c r="U47" s="18"/>
     </row>
     <row r="48" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D48" s="47" t="s">
+      <c r="D48" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="48"/>
+      <c r="E48" s="54"/>
       <c r="F48" s="61" t="s">
         <v>116</v>
       </c>
@@ -3875,8 +3875,8 @@
       <c r="U48" s="63"/>
     </row>
     <row r="49" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D49" s="49"/>
-      <c r="E49" s="50"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="56"/>
       <c r="F49" s="64"/>
       <c r="G49" s="62"/>
       <c r="H49" s="62"/>
@@ -3895,8 +3895,8 @@
       <c r="U49" s="63"/>
     </row>
     <row r="50" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D50" s="49"/>
-      <c r="E50" s="50"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="56"/>
       <c r="F50" s="64"/>
       <c r="G50" s="62"/>
       <c r="H50" s="62"/>
@@ -3915,8 +3915,8 @@
       <c r="U50" s="63"/>
     </row>
     <row r="51" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D51" s="59"/>
-      <c r="E51" s="60"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="58"/>
       <c r="F51" s="65"/>
       <c r="G51" s="66"/>
       <c r="H51" s="66"/>
@@ -3936,6 +3936,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D3:E7"/>
+    <mergeCell ref="D10:E12"/>
+    <mergeCell ref="D18:E20"/>
+    <mergeCell ref="D22:E24"/>
+    <mergeCell ref="D26:E28"/>
     <mergeCell ref="F10:U12"/>
     <mergeCell ref="F26:U28"/>
     <mergeCell ref="F30:U32"/>
@@ -3952,11 +3957,6 @@
     <mergeCell ref="F48:U51"/>
     <mergeCell ref="F22:U24"/>
     <mergeCell ref="F18:U20"/>
-    <mergeCell ref="D3:E7"/>
-    <mergeCell ref="D10:E12"/>
-    <mergeCell ref="D18:E20"/>
-    <mergeCell ref="D22:E24"/>
-    <mergeCell ref="D26:E28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F18" r:id="rId1" xr:uid="{36619635-C56A-4186-9BF4-E751CB45AE65}"/>

</xml_diff>